<commit_message>
Added priming file and changed gender reformulated prompt
</commit_message>
<xml_diff>
--- a/data/ANES_2020_multiple_questions_selected_reformulated.xlsx
+++ b/data/ANES_2020_multiple_questions_selected_reformulated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University Code\RSS-1D4D\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{045BD556-B7F0-4E9C-BF8F-CC35F8250F25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B98908-4F17-4916-8E2F-6DEE37F88FEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5E5B915F-D64D-44ED-8197-0044F60AB7BA}"/>
   </bookViews>
@@ -103,12 +103,6 @@
     <t>1. Improves it as a place 2. Worsens it as a place to live 3. Makes no difference</t>
   </si>
   <si>
-    <t>How would this respondent describe the impact on the family as a whole if the man works outside the home and the woman takes care of the home and family?</t>
-  </si>
-  <si>
-    <t>1. Improves the family as a whole 2. Worsens the family as a whole 3. Makes no difference</t>
-  </si>
-  <si>
     <t>How would this respondent describe the state of the economy these days in the United States?</t>
   </si>
   <si>
@@ -140,6 +134,12 @@
   </si>
   <si>
     <t>1. Should be trying 2. Should not be trying 3. Neither of these</t>
+  </si>
+  <si>
+    <t>How would this respondent assess whether it is better, worse, or makes no difference for the family as a whole if the man works outside the home and the woman takes care of the home and family?</t>
+  </si>
+  <si>
+    <t>1. Better 2. Worse 3. Makes no difference</t>
   </si>
 </sst>
 </file>
@@ -529,7 +529,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -554,10 +554,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D2" s="2"/>
     </row>
@@ -566,7 +566,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
@@ -578,10 +578,10 @@
         <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D4" s="2"/>
     </row>
@@ -590,10 +590,10 @@
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D5" s="2"/>
     </row>
@@ -602,10 +602,10 @@
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="D6" s="2"/>
     </row>
@@ -614,7 +614,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>12</v>
@@ -626,7 +626,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>4</v>
@@ -638,7 +638,7 @@
         <v>13</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>14</v>
@@ -662,7 +662,7 @@
         <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>17</v>

</xml_diff>